<commit_message>
feat: try ragas calculation using excel
</commit_message>
<xml_diff>
--- a/test/adaptive/results/score_ragas_adaptive_20241227071640_vdb1000200_optimization.xlsx
+++ b/test/adaptive/results/score_ragas_adaptive_20241227071640_vdb1000200_optimization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\adaptive\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4104BD-2A04-4830-8C9F-345F1C7F977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41DA136-880B-4C1C-9DAF-F461B7F9E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
@@ -1011,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1019,6 +1019,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,32 +2783,32 @@
         <v>0.91020739921170912</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E51" s="2">
-        <v>0.99999999989999999</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="E51" s="5">
+        <v>0.99999999989999999</v>
+      </c>
+      <c r="F51" s="5">
         <v>0.5</v>
       </c>
-      <c r="G51" s="2">
-        <v>1</v>
-      </c>
-      <c r="H51" s="2">
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
+      <c r="H51" s="5">
         <v>0</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="5">
         <v>0.624999999975</v>
       </c>
     </row>

</xml_diff>